<commit_message>
Mise a jour map labyrinthe excel
</commit_message>
<xml_diff>
--- a/schemaLabyritnthe.xlsx
+++ b/schemaLabyritnthe.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GOUVEIAA_INFO\Desktop\Lost'n Furious\Lost-n-Furious\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrateur\Documents\Lost-n-Furious\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -185,24 +185,59 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -486,14 +521,15 @@
   <dimension ref="A1:S19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q2" sqref="Q2"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.28515625" style="1" customWidth="1"/>
-    <col min="2" max="18" width="4.28515625" customWidth="1"/>
-    <col min="19" max="33" width="3.28515625" customWidth="1"/>
+    <col min="2" max="18" width="4.28515625" style="2" customWidth="1"/>
+    <col min="19" max="33" width="3.28515625" style="2" customWidth="1"/>
+    <col min="34" max="16384" width="11.42578125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -943,7 +979,7 @@
       <c r="S17" s="1"/>
     </row>
     <row r="18" spans="2:19" s="1" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I18" s="2"/>
+      <c r="I18" s="17"/>
     </row>
     <row r="19" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B19" s="1"/>

</xml_diff>

<commit_message>
Mise a jour du fichier excel
</commit_message>
<xml_diff>
--- a/schemaLabyritnthe.xlsx
+++ b/schemaLabyritnthe.xlsx
@@ -1,20 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrateur\Documents\Lost-n-Furious\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programmation\C#\Lost-n-Furious\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11880"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11880" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
+    <sheet name="LabyrintheMoyen" sheetId="1" r:id="rId1"/>
+    <sheet name="LabyrinthePetit" sheetId="2" r:id="rId2"/>
+    <sheet name="LabyrintheGrand" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -520,19 +522,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.28515625" style="1" customWidth="1"/>
-    <col min="2" max="18" width="4.28515625" style="2" customWidth="1"/>
-    <col min="19" max="33" width="3.28515625" style="2" customWidth="1"/>
-    <col min="34" max="16384" width="11.42578125" style="2"/>
+    <col min="1" max="1" width="4.33203125" style="1" customWidth="1"/>
+    <col min="2" max="18" width="4.33203125" style="2" customWidth="1"/>
+    <col min="19" max="33" width="3.33203125" style="2" customWidth="1"/>
+    <col min="34" max="16384" width="11.44140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -556,7 +558,7 @@
       <c r="R1" s="1"/>
       <c r="S1" s="1"/>
     </row>
-    <row r="2" spans="1:19" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="3">
         <v>40</v>
       </c>
@@ -623,7 +625,7 @@
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>
     </row>
-    <row r="3" spans="1:19" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="6">
         <f>B2+30</f>
         <v>70</v>
@@ -646,7 +648,7 @@
       <c r="R3" s="1"/>
       <c r="S3" s="1"/>
     </row>
-    <row r="4" spans="1:19" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="6">
         <f t="shared" ref="B4:B17" si="1">B3+30</f>
         <v>100</v>
@@ -669,7 +671,7 @@
       <c r="R4" s="1"/>
       <c r="S4" s="1"/>
     </row>
-    <row r="5" spans="1:19" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="6">
         <f t="shared" si="1"/>
         <v>130</v>
@@ -692,7 +694,7 @@
       <c r="R5" s="1"/>
       <c r="S5" s="1"/>
     </row>
-    <row r="6" spans="1:19" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="6">
         <f t="shared" si="1"/>
         <v>160</v>
@@ -715,7 +717,7 @@
       <c r="R6" s="1"/>
       <c r="S6" s="1"/>
     </row>
-    <row r="7" spans="1:19" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="6">
         <f t="shared" si="1"/>
         <v>190</v>
@@ -738,7 +740,7 @@
       <c r="R7" s="1"/>
       <c r="S7" s="1"/>
     </row>
-    <row r="8" spans="1:19" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="6">
         <f t="shared" si="1"/>
         <v>220</v>
@@ -761,7 +763,7 @@
       <c r="R8" s="1"/>
       <c r="S8" s="1"/>
     </row>
-    <row r="9" spans="1:19" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="6">
         <f t="shared" si="1"/>
         <v>250</v>
@@ -784,7 +786,7 @@
       <c r="R9" s="1"/>
       <c r="S9" s="1"/>
     </row>
-    <row r="10" spans="1:19" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="6">
         <f t="shared" si="1"/>
         <v>280</v>
@@ -807,7 +809,7 @@
       <c r="R10" s="1"/>
       <c r="S10" s="1"/>
     </row>
-    <row r="11" spans="1:19" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="6">
         <f t="shared" si="1"/>
         <v>310</v>
@@ -830,7 +832,7 @@
       <c r="R11" s="1"/>
       <c r="S11" s="1"/>
     </row>
-    <row r="12" spans="1:19" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="6">
         <f t="shared" si="1"/>
         <v>340</v>
@@ -853,7 +855,7 @@
       <c r="R12" s="1"/>
       <c r="S12" s="1"/>
     </row>
-    <row r="13" spans="1:19" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="6">
         <f t="shared" si="1"/>
         <v>370</v>
@@ -876,7 +878,7 @@
       <c r="R13" s="1"/>
       <c r="S13" s="1"/>
     </row>
-    <row r="14" spans="1:19" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>3</v>
       </c>
@@ -902,7 +904,7 @@
       <c r="R14" s="1"/>
       <c r="S14" s="1"/>
     </row>
-    <row r="15" spans="1:19" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>0</v>
       </c>
@@ -932,7 +934,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:19" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:19" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B16" s="6">
         <f t="shared" si="1"/>
         <v>460</v>
@@ -955,7 +957,7 @@
       <c r="R16" s="1"/>
       <c r="S16" s="1"/>
     </row>
-    <row r="17" spans="2:19" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:19" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B17" s="6">
         <f t="shared" si="1"/>
         <v>490</v>
@@ -978,10 +980,10 @@
       <c r="R17" s="1"/>
       <c r="S17" s="1"/>
     </row>
-    <row r="18" spans="2:19" s="1" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:19" s="1" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="I18" s="17"/>
     </row>
-    <row r="19" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
@@ -1005,4 +1007,28 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>